<commit_message>
Final commit for Portuguese Banking Project
</commit_message>
<xml_diff>
--- a/Code/Portuguese_Bank_Marketing_Project/results_final_20_input.xlsx
+++ b/Code/Portuguese_Bank_Marketing_Project/results_final_20_input.xlsx
@@ -52,19 +52,28 @@
     <t>XGB</t>
   </si>
   <si>
+    <t>StackingCV</t>
+  </si>
+  <si>
     <t>Stacking (SGD)</t>
   </si>
   <si>
     <t>Random Forest</t>
   </si>
   <si>
-    <t>StackingCV</t>
+    <t>Voting</t>
   </si>
   <si>
     <t>Stacking (SVC)</t>
   </si>
   <si>
-    <t>Voting</t>
+    <t>SVM (SVC)</t>
+  </si>
+  <si>
+    <t>Vecstack</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
   </si>
   <si>
     <t>Decision Tree</t>
@@ -73,25 +82,16 @@
     <t>Stacking (Logistic)</t>
   </si>
   <si>
-    <t>SVM (SVC)</t>
-  </si>
-  <si>
-    <t>Vecstack</t>
-  </si>
-  <si>
-    <t>Logistic Regression</t>
-  </si>
-  <si>
     <t>Gaussian Naive-Bayes</t>
   </si>
   <si>
     <t>Bernoulli Naive-Bayes</t>
   </si>
   <si>
+    <t>Full</t>
+  </si>
+  <si>
     <t>Reduced</t>
-  </si>
-  <si>
-    <t>Full</t>
   </si>
   <si>
     <t>Default</t>
@@ -510,109 +510,109 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>0.9514610922622305</v>
+        <v>0.9514063697055927</v>
       </c>
       <c r="F2">
-        <v>0.951195437595964</v>
+        <v>0.9545953059881553</v>
       </c>
       <c r="G2">
-        <v>0.9515085024684586</v>
+        <v>0.9483547613859229</v>
       </c>
       <c r="H2">
-        <v>0.9930124197562735</v>
+        <v>0.9933575380926222</v>
       </c>
       <c r="I2">
-        <v>8673</v>
+        <v>8704</v>
       </c>
       <c r="J2">
-        <v>8714</v>
+        <v>8682</v>
       </c>
       <c r="K2">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c r="L2">
-        <v>445</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3">
-        <v>0.9541972200941228</v>
+        <v>0.9533216591879172</v>
       </c>
       <c r="F3">
-        <v>0.9645755648168458</v>
+        <v>0.9634788330774292</v>
       </c>
       <c r="G3">
-        <v>0.9447846170372758</v>
+        <v>0.9441160666308437</v>
       </c>
       <c r="H3">
-        <v>0.9926731707793867</v>
+        <v>0.9931383833972925</v>
       </c>
       <c r="I3">
-        <v>8795</v>
+        <v>8785</v>
       </c>
       <c r="J3">
-        <v>8642</v>
+        <v>8636</v>
       </c>
       <c r="K3">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="L3">
-        <v>323</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4">
-        <v>0.9497646930064573</v>
+        <v>0.9532669366312794</v>
       </c>
       <c r="F4">
-        <v>0.9744461504715947</v>
+        <v>0.9639175257731959</v>
       </c>
       <c r="G4">
-        <v>0.9284221525600836</v>
+        <v>0.9436332402834443</v>
       </c>
       <c r="H4">
-        <v>0.9925624914295375</v>
+        <v>0.9931375449173695</v>
       </c>
       <c r="I4">
-        <v>8885</v>
+        <v>8789</v>
       </c>
       <c r="J4">
-        <v>8471</v>
+        <v>8631</v>
       </c>
       <c r="K4">
-        <v>685</v>
+        <v>525</v>
       </c>
       <c r="L4">
-        <v>233</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -621,112 +621,112 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
-        <v>0.9523366531684361</v>
+        <v>0.9504760862427493</v>
       </c>
       <c r="F5">
-        <v>0.9647949111647292</v>
+        <v>0.9754332090370695</v>
       </c>
       <c r="G5">
-        <v>0.9411575906708035</v>
+        <v>0.9288772845953003</v>
       </c>
       <c r="H5">
-        <v>0.992558322986491</v>
+        <v>0.9922658432218865</v>
       </c>
       <c r="I5">
-        <v>8797</v>
+        <v>8894</v>
       </c>
       <c r="J5">
-        <v>8606</v>
+        <v>8475</v>
       </c>
       <c r="K5">
-        <v>550</v>
+        <v>681</v>
       </c>
       <c r="L5">
-        <v>321</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
       <c r="E6">
-        <v>0.9553463937835176</v>
+        <v>0.9447302177957754</v>
       </c>
       <c r="F6">
-        <v>0.954375959640272</v>
+        <v>0.9599692915112963</v>
       </c>
       <c r="G6">
-        <v>0.9560536145902</v>
+        <v>0.931368376250266</v>
       </c>
       <c r="H6">
-        <v>0.9867794953999075</v>
+        <v>0.9907880523031318</v>
       </c>
       <c r="I6">
-        <v>8702</v>
+        <v>8753</v>
       </c>
       <c r="J6">
-        <v>8756</v>
+        <v>8511</v>
       </c>
       <c r="K6">
-        <v>400</v>
+        <v>645</v>
       </c>
       <c r="L6">
-        <v>416</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
       </c>
       <c r="E7">
-        <v>0.9326365327788114</v>
+        <v>0.9541972200941228</v>
       </c>
       <c r="F7">
-        <v>0.9697302039921035</v>
+        <v>0.9598596183373547</v>
       </c>
       <c r="G7">
-        <v>0.9025211799530468</v>
+        <v>0.9489320177816328</v>
       </c>
       <c r="H7">
-        <v>0.986047131100217</v>
+        <v>0.9770402396576855</v>
       </c>
       <c r="I7">
-        <v>8842</v>
+        <v>8752</v>
       </c>
       <c r="J7">
-        <v>8201</v>
+        <v>8685</v>
       </c>
       <c r="K7">
-        <v>955</v>
+        <v>471</v>
       </c>
       <c r="L7">
-        <v>276</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -735,112 +735,112 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8">
-        <v>0.8999671664660173</v>
+        <v>0.9111232279171211</v>
       </c>
       <c r="F8">
-        <v>0.951195437595964</v>
+        <v>0.9393939393939394</v>
       </c>
       <c r="G8">
-        <v>0.8624701670644391</v>
+        <v>0.8902564102564102</v>
       </c>
       <c r="H8">
-        <v>0.9568584770943096</v>
+        <v>0.9513557870700727</v>
       </c>
       <c r="I8">
-        <v>8673</v>
+        <v>868</v>
       </c>
       <c r="J8">
-        <v>7773</v>
+        <v>803</v>
       </c>
       <c r="K8">
-        <v>1383</v>
+        <v>107</v>
       </c>
       <c r="L8">
-        <v>445</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
       <c r="E9">
-        <v>0.8969027032942979</v>
+        <v>0.9473021779577542</v>
       </c>
       <c r="F9">
-        <v>0.923009431892959</v>
+        <v>0.9787234042553191</v>
       </c>
       <c r="G9">
-        <v>0.8768493436132527</v>
+        <v>0.9206643969875168</v>
       </c>
       <c r="H9">
-        <v>0.9561970122612595</v>
+        <v>0.9473673814636141</v>
       </c>
       <c r="I9">
-        <v>8416</v>
+        <v>8924</v>
       </c>
       <c r="J9">
-        <v>7974</v>
+        <v>8387</v>
       </c>
       <c r="K9">
-        <v>1182</v>
+        <v>769</v>
       </c>
       <c r="L9">
-        <v>702</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10">
-        <v>0.9127589967284624</v>
+        <v>0.8752872934223487</v>
       </c>
       <c r="F10">
-        <v>0.9491341991341992</v>
+        <v>0.8895591138407546</v>
       </c>
       <c r="G10">
-        <v>0.8858585858585859</v>
+        <v>0.8644356815517426</v>
       </c>
       <c r="H10">
-        <v>0.9543587365015935</v>
+        <v>0.9349048507357206</v>
       </c>
       <c r="I10">
-        <v>877</v>
+        <v>8111</v>
       </c>
       <c r="J10">
-        <v>797</v>
+        <v>7884</v>
       </c>
       <c r="K10">
-        <v>113</v>
+        <v>1272</v>
       </c>
       <c r="L10">
-        <v>47</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -849,36 +849,36 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>0.9463718944949108</v>
+        <v>0.9251942650760644</v>
       </c>
       <c r="F11">
-        <v>0.9787234042553191</v>
+        <v>0.9325509980258828</v>
       </c>
       <c r="G11">
-        <v>0.9190525231719876</v>
+        <v>0.9187466234467855</v>
       </c>
       <c r="H11">
-        <v>0.9464390284710409</v>
+        <v>0.9252095313414691</v>
       </c>
       <c r="I11">
-        <v>8924</v>
+        <v>8503</v>
       </c>
       <c r="J11">
-        <v>8370</v>
+        <v>8404</v>
       </c>
       <c r="K11">
-        <v>786</v>
+        <v>752</v>
       </c>
       <c r="L11">
-        <v>194</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -887,31 +887,31 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12">
-        <v>0.8761081317719164</v>
+        <v>0.9201597898653825</v>
       </c>
       <c r="F12">
-        <v>0.8921912700153543</v>
+        <v>0.9250932221978504</v>
       </c>
       <c r="G12">
-        <v>0.8639549702633815</v>
+        <v>0.9157529041363587</v>
       </c>
       <c r="H12">
-        <v>0.9364567093773967</v>
+        <v>0.9203934883265866</v>
       </c>
       <c r="I12">
-        <v>8135</v>
+        <v>8435</v>
       </c>
       <c r="J12">
-        <v>7875</v>
+        <v>8380</v>
       </c>
       <c r="K12">
-        <v>1281</v>
+        <v>776</v>
       </c>
       <c r="L12">
-        <v>983</v>
+        <v>683</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -922,34 +922,34 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
       </c>
       <c r="E13">
-        <v>0.7672649666192405</v>
+        <v>0.7587282477837365</v>
       </c>
       <c r="F13">
-        <v>0.6766834832200044</v>
+        <v>0.6627549901294143</v>
       </c>
       <c r="G13">
-        <v>0.8254180602006689</v>
+        <v>0.8191676833401111</v>
       </c>
       <c r="H13">
-        <v>0.8642158904690322</v>
+        <v>0.8552142994174434</v>
       </c>
       <c r="I13">
-        <v>6170</v>
+        <v>6043</v>
       </c>
       <c r="J13">
-        <v>7851</v>
+        <v>7822</v>
       </c>
       <c r="K13">
-        <v>1305</v>
+        <v>1334</v>
       </c>
       <c r="L13">
-        <v>2948</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -960,34 +960,34 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
       <c r="E14">
-        <v>0.6812411075845464</v>
+        <v>0.6709532669366313</v>
       </c>
       <c r="F14">
-        <v>0.6471813994296995</v>
+        <v>0.6650581267821891</v>
       </c>
       <c r="G14">
-        <v>0.6935009989422964</v>
+        <v>0.6720602903690569</v>
       </c>
       <c r="H14">
-        <v>0.73773974057527</v>
+        <v>0.7323666294669059</v>
       </c>
       <c r="I14">
-        <v>5901</v>
+        <v>6064</v>
       </c>
       <c r="J14">
-        <v>6548</v>
+        <v>6197</v>
       </c>
       <c r="K14">
-        <v>2608</v>
+        <v>2959</v>
       </c>
       <c r="L14">
-        <v>3217</v>
+        <v>3054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit with changes to Conclusion.
</commit_message>
<xml_diff>
--- a/Code/Portuguese_Bank_Marketing_Project/results_final_20_input.xlsx
+++ b/Code/Portuguese_Bank_Marketing_Project/results_final_20_input.xlsx
@@ -49,55 +49,55 @@
     <t>False_Negatives</t>
   </si>
   <si>
+    <t>StackingCV</t>
+  </si>
+  <si>
+    <t>Stacking (SGD)</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
     <t>XGB</t>
   </si>
   <si>
-    <t>StackingCV</t>
-  </si>
-  <si>
-    <t>Stacking (SGD)</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>Voting</t>
-  </si>
-  <si>
     <t>Stacking (SVC)</t>
   </si>
   <si>
+    <t>Vecstack</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Stacking (Logistic)</t>
+  </si>
+  <si>
     <t>SVM (SVC)</t>
   </si>
   <si>
-    <t>Vecstack</t>
-  </si>
-  <si>
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Decision Tree</t>
-  </si>
-  <si>
-    <t>Stacking (Logistic)</t>
-  </si>
-  <si>
     <t>Gaussian Naive-Bayes</t>
   </si>
   <si>
     <t>Bernoulli Naive-Bayes</t>
   </si>
   <si>
+    <t>Reduced</t>
+  </si>
+  <si>
     <t>Full</t>
   </si>
   <si>
-    <t>Reduced</t>
+    <t>Best</t>
   </si>
   <si>
     <t>Default</t>
-  </si>
-  <si>
-    <t>Best</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -510,109 +510,109 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>0.9514063697055927</v>
+        <v>0.943471598993105</v>
       </c>
       <c r="F2">
-        <v>0.9545953059881553</v>
+        <v>0.9334283834174161</v>
       </c>
       <c r="G2">
-        <v>0.9483547613859229</v>
+        <v>0.9523329976502182</v>
       </c>
       <c r="H2">
-        <v>0.9933575380926222</v>
+        <v>0.9808645226303815</v>
       </c>
       <c r="I2">
-        <v>8704</v>
+        <v>8511</v>
       </c>
       <c r="J2">
-        <v>8682</v>
+        <v>8730</v>
       </c>
       <c r="K2">
-        <v>474</v>
+        <v>426</v>
       </c>
       <c r="L2">
-        <v>414</v>
+        <v>607</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>0.9533216591879172</v>
+        <v>0.9413921418408668</v>
       </c>
       <c r="F3">
-        <v>0.9634788330774292</v>
+        <v>0.928054397894275</v>
       </c>
       <c r="G3">
-        <v>0.9441160666308437</v>
+        <v>0.9532499718373324</v>
       </c>
       <c r="H3">
-        <v>0.9931383833972925</v>
+        <v>0.9801420883286375</v>
       </c>
       <c r="I3">
-        <v>8785</v>
+        <v>8462</v>
       </c>
       <c r="J3">
-        <v>8636</v>
+        <v>8741</v>
       </c>
       <c r="K3">
-        <v>520</v>
+        <v>415</v>
       </c>
       <c r="L3">
-        <v>333</v>
+        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4">
-        <v>0.9532669366312794</v>
+        <v>0.9391485170187152</v>
       </c>
       <c r="F4">
-        <v>0.9639175257731959</v>
+        <v>0.9290414564597499</v>
       </c>
       <c r="G4">
-        <v>0.9436332402834443</v>
+        <v>0.9479632945389436</v>
       </c>
       <c r="H4">
-        <v>0.9931375449173695</v>
+        <v>0.9800656968185005</v>
       </c>
       <c r="I4">
-        <v>8789</v>
+        <v>8471</v>
       </c>
       <c r="J4">
-        <v>8631</v>
+        <v>8691</v>
       </c>
       <c r="K4">
-        <v>525</v>
+        <v>465</v>
       </c>
       <c r="L4">
-        <v>329</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -624,66 +624,66 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>0.9504760862427493</v>
+        <v>0.9387654591222502</v>
       </c>
       <c r="F5">
-        <v>0.9754332090370695</v>
+        <v>0.9264093002851502</v>
       </c>
       <c r="G5">
-        <v>0.9288772845953003</v>
+        <v>0.9496346261944912</v>
       </c>
       <c r="H5">
-        <v>0.9922658432218865</v>
+        <v>0.9781159135727476</v>
       </c>
       <c r="I5">
-        <v>8894</v>
+        <v>8447</v>
       </c>
       <c r="J5">
-        <v>8475</v>
+        <v>8708</v>
       </c>
       <c r="K5">
-        <v>681</v>
+        <v>448</v>
       </c>
       <c r="L5">
-        <v>224</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
       <c r="E6">
-        <v>0.9447302177957754</v>
+        <v>0.9404071358213856</v>
       </c>
       <c r="F6">
-        <v>0.9599692915112963</v>
+        <v>0.911274402281202</v>
       </c>
       <c r="G6">
-        <v>0.931368376250266</v>
+        <v>0.967400162999185</v>
       </c>
       <c r="H6">
-        <v>0.9907880523031318</v>
+        <v>0.9751876601915893</v>
       </c>
       <c r="I6">
-        <v>8753</v>
+        <v>8309</v>
       </c>
       <c r="J6">
-        <v>8511</v>
+        <v>8876</v>
       </c>
       <c r="K6">
-        <v>645</v>
+        <v>280</v>
       </c>
       <c r="L6">
-        <v>365</v>
+        <v>809</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -694,39 +694,39 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>0.9541972200941228</v>
+        <v>0.9466455072781</v>
       </c>
       <c r="F7">
-        <v>0.9598596183373547</v>
+        <v>0.9224610660232507</v>
       </c>
       <c r="G7">
-        <v>0.9489320177816328</v>
+        <v>0.9691208664592695</v>
       </c>
       <c r="H7">
-        <v>0.9770402396576855</v>
+        <v>0.9691942715818264</v>
       </c>
       <c r="I7">
-        <v>8752</v>
+        <v>8411</v>
       </c>
       <c r="J7">
-        <v>8685</v>
+        <v>8888</v>
       </c>
       <c r="K7">
-        <v>471</v>
+        <v>268</v>
       </c>
       <c r="L7">
-        <v>366</v>
+        <v>707</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -738,71 +738,71 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.9111232279171211</v>
+        <v>0.9383824012257853</v>
       </c>
       <c r="F8">
-        <v>0.9393939393939394</v>
+        <v>0.9354025005483658</v>
       </c>
       <c r="G8">
-        <v>0.8902564102564102</v>
+        <v>0.9407677035076109</v>
       </c>
       <c r="H8">
-        <v>0.9513557870700727</v>
+        <v>0.9383762175087831</v>
       </c>
       <c r="I8">
-        <v>868</v>
+        <v>8529</v>
       </c>
       <c r="J8">
-        <v>803</v>
+        <v>8619</v>
       </c>
       <c r="K8">
-        <v>107</v>
+        <v>537</v>
       </c>
       <c r="L8">
-        <v>56</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>0.9473021779577542</v>
+        <v>0.8984349348801576</v>
       </c>
       <c r="F9">
-        <v>0.9787234042553191</v>
+        <v>0.8811142794472472</v>
       </c>
       <c r="G9">
-        <v>0.9206643969875168</v>
+        <v>0.9123325005677947</v>
       </c>
       <c r="H9">
-        <v>0.9473673814636141</v>
+        <v>0.9180263876339639</v>
       </c>
       <c r="I9">
-        <v>8924</v>
+        <v>8034</v>
       </c>
       <c r="J9">
-        <v>8387</v>
+        <v>8384</v>
       </c>
       <c r="K9">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="L9">
-        <v>194</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -814,71 +814,71 @@
         <v>26</v>
       </c>
       <c r="E10">
-        <v>0.8752872934223487</v>
+        <v>0.8984349348801576</v>
       </c>
       <c r="F10">
-        <v>0.8895591138407546</v>
+        <v>0.8811142794472472</v>
       </c>
       <c r="G10">
-        <v>0.8644356815517426</v>
+        <v>0.9123325005677947</v>
       </c>
       <c r="H10">
-        <v>0.9349048507357206</v>
+        <v>0.9179473069989308</v>
       </c>
       <c r="I10">
-        <v>8111</v>
+        <v>8034</v>
       </c>
       <c r="J10">
-        <v>7884</v>
+        <v>8384</v>
       </c>
       <c r="K10">
-        <v>1272</v>
+        <v>772</v>
       </c>
       <c r="L10">
-        <v>1007</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11">
-        <v>0.9251942650760644</v>
+        <v>0.7633587786259542</v>
       </c>
       <c r="F11">
-        <v>0.9325509980258828</v>
+        <v>0.6872294372294372</v>
       </c>
       <c r="G11">
-        <v>0.9187466234467855</v>
+        <v>0.8141025641025641</v>
       </c>
       <c r="H11">
-        <v>0.9252095313414691</v>
+        <v>0.8596272774844202</v>
       </c>
       <c r="I11">
-        <v>8503</v>
+        <v>635</v>
       </c>
       <c r="J11">
-        <v>8404</v>
+        <v>765</v>
       </c>
       <c r="K11">
-        <v>752</v>
+        <v>145</v>
       </c>
       <c r="L11">
-        <v>615</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -890,28 +890,28 @@
         <v>27</v>
       </c>
       <c r="E12">
-        <v>0.9201597898653825</v>
+        <v>0.7284119514063697</v>
       </c>
       <c r="F12">
-        <v>0.9250932221978504</v>
+        <v>0.657490677780215</v>
       </c>
       <c r="G12">
-        <v>0.9157529041363587</v>
+        <v>0.7651563497128271</v>
       </c>
       <c r="H12">
-        <v>0.9203934883265866</v>
+        <v>0.7784839295979675</v>
       </c>
       <c r="I12">
-        <v>8435</v>
+        <v>5995</v>
       </c>
       <c r="J12">
-        <v>8380</v>
+        <v>7316</v>
       </c>
       <c r="K12">
-        <v>776</v>
+        <v>1840</v>
       </c>
       <c r="L12">
-        <v>683</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -922,34 +922,34 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13">
-        <v>0.7587282477837365</v>
+        <v>0.6958520302068513</v>
       </c>
       <c r="F13">
-        <v>0.6627549901294143</v>
+        <v>0.5834612853695986</v>
       </c>
       <c r="G13">
-        <v>0.8191676833401111</v>
+        <v>0.751412429378531</v>
       </c>
       <c r="H13">
-        <v>0.8552142994174434</v>
+        <v>0.7514114551785527</v>
       </c>
       <c r="I13">
-        <v>6043</v>
+        <v>5320</v>
       </c>
       <c r="J13">
-        <v>7822</v>
+        <v>7396</v>
       </c>
       <c r="K13">
-        <v>1334</v>
+        <v>1760</v>
       </c>
       <c r="L13">
-        <v>3075</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -960,34 +960,34 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14">
-        <v>0.6709532669366313</v>
+        <v>0.6720477180693882</v>
       </c>
       <c r="F14">
-        <v>0.6650581267821891</v>
+        <v>0.6668128975652555</v>
       </c>
       <c r="G14">
-        <v>0.6720602903690569</v>
+        <v>0.6729385722191478</v>
       </c>
       <c r="H14">
-        <v>0.7323666294669059</v>
+        <v>0.7313179426270831</v>
       </c>
       <c r="I14">
-        <v>6064</v>
+        <v>6080</v>
       </c>
       <c r="J14">
-        <v>6197</v>
+        <v>6201</v>
       </c>
       <c r="K14">
-        <v>2959</v>
+        <v>2955</v>
       </c>
       <c r="L14">
-        <v>3054</v>
+        <v>3038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>